<commit_message>
Added formulas to deal with new morale rules on the number of farmers/plumbers and also based on population size
</commit_message>
<xml_diff>
--- a/SCS Perfect Game.xlsx
+++ b/SCS Perfect Game.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denn0\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\SpaceColonySim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="207" documentId="8_{124DFF72-0B1A-4B90-90AC-EF4BE2CAC000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9367BA29-D762-4B4D-89B4-A7FF992473CC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B60BF2A-BFEB-4E5F-8FE7-70F8E6C32879}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="20376" windowHeight="12816" xr2:uid="{AC332483-67BD-4258-AFD5-EC76FAA49507}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <definedName name="FoodProd">'Turn Data'!$O$6</definedName>
     <definedName name="FoodUse">'Turn Data'!$O$4</definedName>
     <definedName name="IceProd">'Turn Data'!$O$8</definedName>
-    <definedName name="ObjMoraleMods">'Turn Data'!$Z$3:$AA$14</definedName>
+    <definedName name="ObjMoraleMods">'Turn Data'!$AC$3:$AD$14</definedName>
     <definedName name="OreProd">'Turn Data'!$O$7</definedName>
     <definedName name="WaterProd">'Turn Data'!$O$9</definedName>
     <definedName name="WaterUse">'Turn Data'!$O$5</definedName>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>Turn</t>
   </si>
@@ -178,6 +178,15 @@
   </si>
   <si>
     <t>Modifier</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Farmers</t>
+  </si>
+  <si>
+    <t>Plumbers</t>
   </si>
 </sst>
 </file>
@@ -454,91 +463,91 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="26">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="27">
                   <c:v>52</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="28">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="29">
                   <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>67</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>71</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>83</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2472,10 +2481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{363EE1E3-190E-4478-8833-40E787F3C5BD}">
-  <dimension ref="A1:AA33"/>
+  <dimension ref="A1:AD33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2487,14 +2496,17 @@
     <col min="16" max="16" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="11.109375" customWidth="1"/>
+    <col min="19" max="19" width="7.88671875" customWidth="1"/>
+    <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.6640625" customWidth="1"/>
+    <col min="24" max="24" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>19</v>
       </c>
@@ -2530,8 +2542,11 @@
       <c r="Y1" s="17"/>
       <c r="Z1" s="17"/>
       <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="17"/>
+      <c r="AD1" s="17"/>
     </row>
-    <row r="2" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2567,12 +2582,15 @@
       <c r="W2" s="17"/>
       <c r="X2" s="17"/>
       <c r="Y2" s="17"/>
-      <c r="Z2" s="15" t="s">
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="17"/>
+      <c r="AB2" s="17"/>
+      <c r="AC2" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="AA2" s="3"/>
+      <c r="AD2" s="3"/>
     </row>
-    <row r="3" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -2628,34 +2646,43 @@
         <v>34</v>
       </c>
       <c r="S3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="AA3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="AB3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="AC3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -2712,40 +2739,52 @@
         <v>-10</v>
       </c>
       <c r="S4" s="9">
+        <f>IF(H4=0,-10,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="9">
         <f>IF(E4&gt;2*B4,15,0)</f>
         <v>15</v>
       </c>
-      <c r="T4" s="9">
+      <c r="U4" s="9">
         <f>IF(E4&lt;B4,-15,0)</f>
         <v>0</v>
       </c>
-      <c r="U4" s="9">
+      <c r="V4" s="9">
         <f>IF(E4=0,B4*3,0)</f>
         <v>0</v>
       </c>
-      <c r="V4" s="9">
-        <v>0</v>
-      </c>
       <c r="W4" s="9">
+        <f>IF(K4=0,-20,IF(K4&lt;B4/6,-10,0))</f>
+        <v>-20</v>
+      </c>
+      <c r="X4" s="9">
+        <f>-1 * B4</f>
+        <v>-10</v>
+      </c>
+      <c r="Y4" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="9">
         <f>IF(B4&gt;2*SUM(H4:L4),-1*(B4-2*SUM(H4:L4)*2),0)</f>
         <v>0</v>
       </c>
-      <c r="X4" s="9">
+      <c r="AA4" s="9">
         <f>IF(C4&lt;20,20-C4,0)-IF(C4&gt;80,C4-80,0)</f>
         <v>0</v>
       </c>
-      <c r="Y4" s="9">
-        <f>SUM(P4:X4)</f>
+      <c r="AB4" s="9">
+        <f>SUM(P4:AA4)</f>
+        <v>-35</v>
+      </c>
+      <c r="AC4" s="9">
+        <v>-100</v>
+      </c>
+      <c r="AD4" s="9">
         <v>-5</v>
       </c>
-      <c r="Z4" s="9">
-        <v>-100</v>
-      </c>
-      <c r="AA4" s="9">
-        <v>-5</v>
-      </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -2753,8 +2792,8 @@
         <v>10</v>
       </c>
       <c r="C5" s="10">
-        <f t="shared" ref="C5:C33" si="0">C4+VLOOKUP(Y4,ObjMoraleMods,2)</f>
-        <v>50</v>
+        <f t="shared" ref="C5:C33" si="0">C4+VLOOKUP(AB4,ObjMoraleMods,2)</f>
+        <v>47</v>
       </c>
       <c r="D5" s="11">
         <f t="shared" ref="D5:D33" si="1">D4+H4*FoodProd-_xlfn.FLOOR.MATH(B4/FoodUse)</f>
@@ -2807,40 +2846,52 @@
         <v>0</v>
       </c>
       <c r="S5" s="9">
-        <f t="shared" ref="S5:S32" si="8">IF(E5&gt;2*B5,15,0)</f>
+        <f t="shared" ref="S5:S32" si="8">IF(H5=0,-10,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T5" s="9">
+        <f t="shared" ref="T5:T32" si="9">IF(E5&gt;2*B5,15,0)</f>
         <v>15</v>
       </c>
-      <c r="T5" s="9">
-        <f t="shared" ref="T5:T32" si="9">IF(E5&lt;B5,-15,0)</f>
-        <v>0</v>
-      </c>
       <c r="U5" s="9">
-        <f t="shared" ref="U5:U32" si="10">IF(E5=0,B5*3,0)</f>
+        <f t="shared" ref="U5:U32" si="10">IF(E5&lt;B5,-15,0)</f>
         <v>0</v>
       </c>
       <c r="V5" s="9">
+        <f t="shared" ref="V5:V32" si="11">IF(E5=0,B5*3,0)</f>
         <v>0</v>
       </c>
       <c r="W5" s="9">
-        <f t="shared" ref="W5:W32" si="11">IF(B5&gt;2*SUM(H5:L5),-1*(B5-2*SUM(H5:L5)*2),0)</f>
-        <v>0</v>
+        <f t="shared" ref="W5:W32" si="12">IF(K5=0,-20,IF(K5&lt;B5/6,-10,0))</f>
+        <v>-20</v>
       </c>
       <c r="X5" s="9">
-        <f t="shared" ref="X5:X32" si="12">IF(C5&lt;20,20-C5,0)-IF(C5&gt;80,C5-80,0)</f>
-        <v>0</v>
+        <f t="shared" ref="X5:X32" si="13">-1 * B5</f>
+        <v>-10</v>
       </c>
       <c r="Y5" s="9">
-        <f t="shared" ref="Y5:Y32" si="13">SUM(P5:X5)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Z5" s="9">
+        <f t="shared" ref="Z5:Z32" si="14">IF(B5&gt;2*SUM(H5:L5),-1*(B5-2*SUM(H5:L5)*2),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA5" s="9">
+        <f t="shared" ref="AA5:AA32" si="15">IF(C5&lt;20,20-C5,0)-IF(C5&gt;80,C5-80,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB5" s="9">
+        <f t="shared" ref="AB5:AB32" si="16">SUM(P5:AA5)</f>
+        <v>-25</v>
+      </c>
+      <c r="AC5" s="9">
         <v>-51</v>
       </c>
-      <c r="AA5" s="9">
+      <c r="AD5" s="9">
         <v>-4</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -2849,7 +2900,7 @@
       </c>
       <c r="C6" s="10">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D6" s="11">
         <f t="shared" si="1"/>
@@ -2905,39 +2956,51 @@
       </c>
       <c r="S6" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T6" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U6" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V6" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W6" s="9">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>-20</v>
       </c>
       <c r="X6" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y6" s="9">
-        <f t="shared" si="13"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Z6" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA6" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB6" s="9">
+        <f t="shared" si="16"/>
+        <v>-25</v>
+      </c>
+      <c r="AC6" s="9">
         <v>-41</v>
       </c>
-      <c r="AA6" s="9">
+      <c r="AD6" s="9">
         <v>-3</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -2946,7 +3009,7 @@
       </c>
       <c r="C7" s="10">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D7" s="11">
         <f t="shared" si="1"/>
@@ -3002,39 +3065,51 @@
       </c>
       <c r="S7" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T7" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U7" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V7" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W7" s="9">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>-20</v>
       </c>
       <c r="X7" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y7" s="9">
-        <f t="shared" si="13"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Z7" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA7" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB7" s="9">
+        <f t="shared" si="16"/>
+        <v>-15</v>
+      </c>
+      <c r="AC7" s="9">
         <v>-31</v>
       </c>
-      <c r="AA7" s="9">
+      <c r="AD7" s="9">
         <v>-2</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -3043,7 +3118,7 @@
       </c>
       <c r="C8" s="10">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D8" s="11">
         <f t="shared" si="1"/>
@@ -3099,39 +3174,51 @@
       </c>
       <c r="S8" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T8" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U8" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V8" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W8" s="9">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>-20</v>
       </c>
       <c r="X8" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y8" s="9">
-        <f t="shared" si="13"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Z8" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB8" s="9">
+        <f t="shared" si="16"/>
+        <v>-15</v>
+      </c>
+      <c r="AC8" s="9">
         <v>-21</v>
       </c>
-      <c r="AA8" s="9">
+      <c r="AD8" s="9">
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -3140,7 +3227,7 @@
       </c>
       <c r="C9" s="10">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D9" s="11">
         <f t="shared" si="1"/>
@@ -3196,39 +3283,51 @@
       </c>
       <c r="S9" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T9" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U9" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V9" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W9" s="9">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>-20</v>
       </c>
       <c r="X9" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y9" s="9">
-        <f t="shared" si="13"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Z9" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA9" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB9" s="9">
+        <f t="shared" si="16"/>
+        <v>-15</v>
+      </c>
+      <c r="AC9" s="9">
         <v>-11</v>
       </c>
-      <c r="AA9" s="9">
+      <c r="AD9" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -3237,7 +3336,7 @@
       </c>
       <c r="C10" s="10">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D10" s="11">
         <f t="shared" si="1"/>
@@ -3289,39 +3388,51 @@
       </c>
       <c r="S10" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T10" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U10" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V10" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W10" s="9">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>-20</v>
       </c>
       <c r="X10" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y10" s="9">
-        <f t="shared" si="13"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Z10" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA10" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB10" s="9">
+        <f t="shared" si="16"/>
+        <v>-15</v>
+      </c>
+      <c r="AC10" s="9">
         <v>10</v>
       </c>
-      <c r="AA10" s="9">
+      <c r="AD10" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -3330,7 +3441,7 @@
       </c>
       <c r="C11" s="10">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D11" s="11">
         <f t="shared" si="1"/>
@@ -3382,39 +3493,51 @@
       </c>
       <c r="S11" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T11" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U11" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V11" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W11" s="9">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>-20</v>
       </c>
       <c r="X11" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y11" s="9">
-        <f t="shared" si="13"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Z11" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA11" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB11" s="9">
+        <f t="shared" si="16"/>
+        <v>-15</v>
+      </c>
+      <c r="AC11" s="9">
         <v>20</v>
       </c>
-      <c r="AA11" s="9">
+      <c r="AD11" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -3423,7 +3546,7 @@
       </c>
       <c r="C12" s="10">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D12" s="11">
         <f t="shared" si="1"/>
@@ -3475,39 +3598,51 @@
       </c>
       <c r="S12" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T12" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U12" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V12" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W12" s="9">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>-20</v>
       </c>
       <c r="X12" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y12" s="9">
-        <f t="shared" si="13"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Z12" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA12" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB12" s="9">
+        <f t="shared" si="16"/>
+        <v>-15</v>
+      </c>
+      <c r="AC12" s="9">
         <v>30</v>
       </c>
-      <c r="AA12" s="9">
+      <c r="AD12" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -3516,7 +3651,7 @@
       </c>
       <c r="C13" s="10">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="D13" s="11">
         <f t="shared" si="1"/>
@@ -3566,39 +3701,51 @@
       </c>
       <c r="S13" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T13" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U13" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V13" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W13" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X13" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y13" s="9">
-        <f t="shared" si="13"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Z13" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA13" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB13" s="9">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="AC13" s="9">
         <v>40</v>
       </c>
-      <c r="AA13" s="9">
+      <c r="AD13" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -3607,7 +3754,7 @@
       </c>
       <c r="C14" s="10">
         <f t="shared" si="0"/>
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="D14" s="11">
         <f t="shared" si="1"/>
@@ -3657,39 +3804,51 @@
       </c>
       <c r="S14" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T14" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U14" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V14" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W14" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X14" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y14" s="9">
-        <f t="shared" si="13"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA14" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB14" s="9">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="AC14" s="9">
         <v>50</v>
       </c>
-      <c r="AA14" s="9">
+      <c r="AD14" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -3698,7 +3857,7 @@
       </c>
       <c r="C15" s="10">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="D15" s="11">
         <f t="shared" si="1"/>
@@ -3748,35 +3907,47 @@
       </c>
       <c r="S15" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T15" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U15" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V15" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W15" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X15" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y15" s="9">
-        <f t="shared" si="13"/>
-        <v>15</v>
-      </c>
-      <c r="Z15" s="9"/>
-      <c r="AA15" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z15" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA15" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB15" s="9">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="AC15" s="9"/>
+      <c r="AD15" s="9"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -3785,7 +3956,7 @@
       </c>
       <c r="C16" s="10">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="D16" s="11">
         <f t="shared" si="1"/>
@@ -3835,35 +4006,47 @@
       </c>
       <c r="S16" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T16" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U16" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V16" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W16" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X16" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y16" s="9">
-        <f t="shared" si="13"/>
-        <v>25</v>
-      </c>
-      <c r="Z16" s="9"/>
-      <c r="AA16" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z16" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA16" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB16" s="9">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="AC16" s="9"/>
+      <c r="AD16" s="9"/>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>14</v>
       </c>
@@ -3872,7 +4055,7 @@
       </c>
       <c r="C17" s="10">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="D17" s="11">
         <f t="shared" si="1"/>
@@ -3922,35 +4105,47 @@
       </c>
       <c r="S17" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T17" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U17" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V17" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W17" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X17" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y17" s="9">
-        <f t="shared" si="13"/>
-        <v>25</v>
-      </c>
-      <c r="Z17" s="9"/>
-      <c r="AA17" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z17" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA17" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB17" s="9">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="AC17" s="9"/>
+      <c r="AD17" s="9"/>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>15</v>
       </c>
@@ -3959,7 +4154,7 @@
       </c>
       <c r="C18" s="10">
         <f t="shared" si="0"/>
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D18" s="11">
         <f t="shared" si="1"/>
@@ -4009,35 +4204,47 @@
       </c>
       <c r="S18" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T18" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U18" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V18" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W18" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X18" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y18" s="9">
-        <f t="shared" si="13"/>
-        <v>25</v>
-      </c>
-      <c r="Z18" s="9"/>
-      <c r="AA18" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z18" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA18" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB18" s="9">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="AC18" s="9"/>
+      <c r="AD18" s="9"/>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>16</v>
       </c>
@@ -4046,7 +4253,7 @@
       </c>
       <c r="C19" s="10">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="D19" s="11">
         <f t="shared" si="1"/>
@@ -4096,35 +4303,47 @@
       </c>
       <c r="S19" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T19" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U19" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V19" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W19" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X19" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y19" s="9">
-        <f t="shared" si="13"/>
-        <v>25</v>
-      </c>
-      <c r="Z19" s="9"/>
-      <c r="AA19" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z19" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA19" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB19" s="9">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="AC19" s="9"/>
+      <c r="AD19" s="9"/>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <v>17</v>
       </c>
@@ -4133,7 +4352,7 @@
       </c>
       <c r="C20" s="10">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="D20" s="11">
         <f t="shared" si="1"/>
@@ -4183,35 +4402,47 @@
       </c>
       <c r="S20" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T20" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U20" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V20" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W20" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X20" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y20" s="9">
-        <f t="shared" si="13"/>
-        <v>25</v>
-      </c>
-      <c r="Z20" s="9"/>
-      <c r="AA20" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z20" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA20" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB20" s="9">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="AC20" s="9"/>
+      <c r="AD20" s="9"/>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
         <v>18</v>
       </c>
@@ -4220,7 +4451,7 @@
       </c>
       <c r="C21" s="10">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="D21" s="11">
         <f t="shared" si="1"/>
@@ -4270,35 +4501,47 @@
       </c>
       <c r="S21" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T21" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U21" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V21" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W21" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X21" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y21" s="9">
-        <f t="shared" si="13"/>
-        <v>25</v>
-      </c>
-      <c r="Z21" s="9"/>
-      <c r="AA21" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z21" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA21" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB21" s="9">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="AC21" s="9"/>
+      <c r="AD21" s="9"/>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
         <v>19</v>
       </c>
@@ -4307,7 +4550,7 @@
       </c>
       <c r="C22" s="10">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="D22" s="11">
         <f t="shared" si="1"/>
@@ -4357,35 +4600,47 @@
       </c>
       <c r="S22" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T22" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U22" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V22" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W22" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X22" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y22" s="9">
-        <f t="shared" si="13"/>
-        <v>25</v>
-      </c>
-      <c r="Z22" s="9"/>
-      <c r="AA22" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z22" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA22" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB22" s="9">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="AC22" s="9"/>
+      <c r="AD22" s="9"/>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" s="9">
         <v>20</v>
       </c>
@@ -4394,7 +4649,7 @@
       </c>
       <c r="C23" s="10">
         <f t="shared" si="0"/>
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="D23" s="11">
         <f t="shared" si="1"/>
@@ -4444,35 +4699,47 @@
       </c>
       <c r="S23" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T23" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U23" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V23" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W23" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X23" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y23" s="9">
-        <f t="shared" si="13"/>
-        <v>25</v>
-      </c>
-      <c r="Z23" s="9"/>
-      <c r="AA23" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z23" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA23" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB23" s="9">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="AC23" s="9"/>
+      <c r="AD23" s="9"/>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
         <v>21</v>
       </c>
@@ -4481,7 +4748,7 @@
       </c>
       <c r="C24" s="10">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="D24" s="11">
         <f t="shared" si="1"/>
@@ -4531,35 +4798,47 @@
       </c>
       <c r="S24" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T24" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U24" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V24" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W24" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X24" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y24" s="9">
-        <f t="shared" si="13"/>
-        <v>25</v>
-      </c>
-      <c r="Z24" s="9"/>
-      <c r="AA24" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z24" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA24" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB24" s="9">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="AC24" s="9"/>
+      <c r="AD24" s="9"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" s="9">
         <v>22</v>
       </c>
@@ -4568,7 +4847,7 @@
       </c>
       <c r="C25" s="10">
         <f t="shared" si="0"/>
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="D25" s="11">
         <f t="shared" si="1"/>
@@ -4618,35 +4897,47 @@
       </c>
       <c r="S25" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T25" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U25" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V25" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W25" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X25" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y25" s="9">
-        <f t="shared" si="13"/>
-        <v>25</v>
-      </c>
-      <c r="Z25" s="9"/>
-      <c r="AA25" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z25" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA25" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB25" s="9">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="AC25" s="9"/>
+      <c r="AD25" s="9"/>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A26" s="9">
         <v>23</v>
       </c>
@@ -4655,7 +4946,7 @@
       </c>
       <c r="C26" s="10">
         <f t="shared" si="0"/>
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="D26" s="11">
         <f t="shared" si="1"/>
@@ -4705,35 +4996,47 @@
       </c>
       <c r="S26" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T26" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U26" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V26" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W26" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X26" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y26" s="9">
-        <f t="shared" si="13"/>
-        <v>25</v>
-      </c>
-      <c r="Z26" s="9"/>
-      <c r="AA26" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z26" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA26" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB26" s="9">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="AC26" s="9"/>
+      <c r="AD26" s="9"/>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
         <v>24</v>
       </c>
@@ -4742,7 +5045,7 @@
       </c>
       <c r="C27" s="10">
         <f t="shared" si="0"/>
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="D27" s="11">
         <f t="shared" si="1"/>
@@ -4792,35 +5095,47 @@
       </c>
       <c r="S27" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T27" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U27" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V27" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W27" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X27" s="9">
-        <f t="shared" si="12"/>
-        <v>-1</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y27" s="9">
-        <f t="shared" si="13"/>
-        <v>24</v>
-      </c>
-      <c r="Z27" s="9"/>
-      <c r="AA27" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z27" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA27" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB27" s="9">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="AC27" s="9"/>
+      <c r="AD27" s="9"/>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" s="9">
         <v>25</v>
       </c>
@@ -4829,7 +5144,7 @@
       </c>
       <c r="C28" s="10">
         <f t="shared" si="0"/>
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="D28" s="11">
         <f t="shared" si="1"/>
@@ -4879,35 +5194,47 @@
       </c>
       <c r="S28" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T28" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U28" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V28" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W28" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X28" s="9">
-        <f t="shared" si="12"/>
-        <v>-3</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y28" s="9">
-        <f t="shared" si="13"/>
-        <v>22</v>
-      </c>
-      <c r="Z28" s="9"/>
-      <c r="AA28" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z28" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA28" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB28" s="9">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="AC28" s="9"/>
+      <c r="AD28" s="9"/>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29" s="9">
         <v>26</v>
       </c>
@@ -4916,7 +5243,7 @@
       </c>
       <c r="C29" s="10">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="D29" s="11">
         <f t="shared" si="1"/>
@@ -4966,35 +5293,47 @@
       </c>
       <c r="S29" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T29" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U29" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V29" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W29" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X29" s="9">
-        <f t="shared" si="12"/>
-        <v>-5</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y29" s="9">
-        <f t="shared" si="13"/>
-        <v>20</v>
-      </c>
-      <c r="Z29" s="9"/>
-      <c r="AA29" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z29" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA29" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB29" s="9">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="AC29" s="9"/>
+      <c r="AD29" s="9"/>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A30" s="9">
         <v>27</v>
       </c>
@@ -5003,7 +5342,7 @@
       </c>
       <c r="C30" s="10">
         <f t="shared" si="0"/>
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="D30" s="11">
         <f t="shared" si="1"/>
@@ -5053,35 +5392,47 @@
       </c>
       <c r="S30" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T30" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U30" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V30" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W30" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X30" s="9">
-        <f t="shared" si="12"/>
-        <v>-7</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y30" s="9">
-        <f t="shared" si="13"/>
-        <v>18</v>
-      </c>
-      <c r="Z30" s="9"/>
-      <c r="AA30" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z30" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA30" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB30" s="9">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="AC30" s="9"/>
+      <c r="AD30" s="9"/>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A31" s="9">
         <v>28</v>
       </c>
@@ -5090,7 +5441,7 @@
       </c>
       <c r="C31" s="10">
         <f t="shared" si="0"/>
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="D31" s="11">
         <f t="shared" si="1"/>
@@ -5140,35 +5491,47 @@
       </c>
       <c r="S31" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T31" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U31" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V31" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W31" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X31" s="9">
-        <f t="shared" si="12"/>
-        <v>-8</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y31" s="9">
-        <f t="shared" si="13"/>
-        <v>17</v>
-      </c>
-      <c r="Z31" s="9"/>
-      <c r="AA31" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z31" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA31" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB31" s="9">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="AC31" s="9"/>
+      <c r="AD31" s="9"/>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A32" s="9">
         <v>29</v>
       </c>
@@ -5177,7 +5540,7 @@
       </c>
       <c r="C32" s="10">
         <f t="shared" si="0"/>
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="D32" s="11">
         <f t="shared" si="1"/>
@@ -5227,35 +5590,47 @@
       </c>
       <c r="S32" s="9">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T32" s="9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U32" s="9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V32" s="9">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W32" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X32" s="9">
-        <f t="shared" si="12"/>
-        <v>-9</v>
+        <f t="shared" si="13"/>
+        <v>-10</v>
       </c>
       <c r="Y32" s="9">
-        <f t="shared" si="13"/>
-        <v>16</v>
-      </c>
-      <c r="Z32" s="9"/>
-      <c r="AA32" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z32" s="9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AA32" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB32" s="9">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="AC32" s="9"/>
+      <c r="AD32" s="9"/>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A33" s="9">
         <v>30</v>
       </c>
@@ -5264,7 +5639,7 @@
       </c>
       <c r="C33" s="10">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="D33" s="11">
         <f t="shared" si="1"/>
@@ -5302,6 +5677,9 @@
       <c r="Y33" s="9"/>
       <c r="Z33" s="9"/>
       <c r="AA33" s="9"/>
+      <c r="AB33" s="9"/>
+      <c r="AC33" s="9"/>
+      <c r="AD33" s="9"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
@@ -5310,10 +5688,10 @@
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="H1:M1"/>
-    <mergeCell ref="P2:Y2"/>
+    <mergeCell ref="P2:AB2"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:AA1"/>
+    <mergeCell ref="P1:AD1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>